<commit_message>
Uploading the files for London 2012 page. Miscellaneous fixes on different pages.
</commit_message>
<xml_diff>
--- a/Final_Project/Source Data/Olympic Athletes by Country - London 2012.xlsx
+++ b/Final_Project/Source Data/Olympic Athletes by Country - London 2012.xlsx
@@ -16,621 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
   <si>
-    <t> Great Britain</t>
-  </si>
-  <si>
-    <t> United States</t>
-  </si>
-  <si>
-    <t> Russia</t>
-  </si>
-  <si>
-    <t> Australia</t>
-  </si>
-  <si>
-    <t> China</t>
-  </si>
-  <si>
-    <t> Germany</t>
-  </si>
-  <si>
-    <t> France</t>
-  </si>
-  <si>
-    <t> Japan</t>
-  </si>
-  <si>
-    <t> Italy</t>
-  </si>
-  <si>
-    <t> Spain</t>
-  </si>
-  <si>
-    <t> Canada</t>
-  </si>
-  <si>
-    <t> Brazil</t>
-  </si>
-  <si>
-    <t> South Korea</t>
-  </si>
-  <si>
-    <t> Ukraine</t>
-  </si>
-  <si>
-    <t> Poland</t>
-  </si>
-  <si>
-    <t> New Zealand</t>
-  </si>
-  <si>
-    <t> Netherlands</t>
-  </si>
-  <si>
-    <t> Belarus</t>
-  </si>
-  <si>
-    <t> Hungary</t>
-  </si>
-  <si>
-    <t> Argentina</t>
-  </si>
-  <si>
-    <t> Sweden</t>
-  </si>
-  <si>
-    <t> Czech Republic</t>
-  </si>
-  <si>
-    <t> South Africa</t>
-  </si>
-  <si>
-    <t> Belgium</t>
-  </si>
-  <si>
-    <t> Serbia</t>
-  </si>
-  <si>
-    <t> Kazakhstan</t>
-  </si>
-  <si>
-    <t> Turkey</t>
-  </si>
-  <si>
-    <t> Denmark</t>
-  </si>
-  <si>
-    <t> Egypt</t>
-  </si>
-  <si>
-    <t> Cuba</t>
-  </si>
-  <si>
-    <t> Croatia</t>
-  </si>
-  <si>
-    <t> Colombia</t>
-  </si>
-  <si>
-    <t> Greece</t>
-  </si>
-  <si>
-    <t> Romania</t>
-  </si>
-  <si>
-    <t> Mexico</t>
-  </si>
-  <si>
-    <t> Switzerland</t>
-  </si>
-  <si>
-    <t> India</t>
-  </si>
-  <si>
-    <t> Tunisia</t>
-  </si>
-  <si>
-    <t> Portugal</t>
-  </si>
-  <si>
-    <t> Austria</t>
-  </si>
-  <si>
-    <t> Venezuela</t>
-  </si>
-  <si>
-    <t> Morocco</t>
-  </si>
-  <si>
-    <t> Ireland</t>
-  </si>
-  <si>
-    <t> Slovenia</t>
-  </si>
-  <si>
-    <t> Norway</t>
-  </si>
-  <si>
-    <t> Bulgaria</t>
-  </si>
-  <si>
-    <t> Lithuania</t>
-  </si>
-  <si>
-    <t> Finland</t>
-  </si>
-  <si>
-    <t> Nigeria</t>
-  </si>
-  <si>
-    <t> Uzbekistan</t>
-  </si>
-  <si>
-    <t> Azerbaijan</t>
-  </si>
-  <si>
-    <t> Iran</t>
-  </si>
-  <si>
-    <t> North Korea</t>
-  </si>
-  <si>
-    <t> Jamaica</t>
-  </si>
-  <si>
-    <t> Kenya</t>
-  </si>
-  <si>
-    <t> Slovakia</t>
-  </si>
-  <si>
-    <t> Latvia</t>
-  </si>
-  <si>
-    <t> Chinese Taipei</t>
-  </si>
-  <si>
-    <t> Algeria</t>
-  </si>
-  <si>
-    <t> Hong Kong</t>
-  </si>
-  <si>
-    <t> Israel</t>
-  </si>
-  <si>
-    <t> Thailand</t>
-  </si>
-  <si>
-    <t> Ecuador</t>
-  </si>
-  <si>
-    <t> Chile</t>
-  </si>
-  <si>
-    <t> Dominican Republic</t>
-  </si>
-  <si>
-    <t> Ethiopia</t>
-  </si>
-  <si>
-    <t> Georgia</t>
-  </si>
-  <si>
-    <t> Angola</t>
-  </si>
-  <si>
-    <t> Cameroon</t>
-  </si>
-  <si>
-    <t> Estonia</t>
-  </si>
-  <si>
-    <t> Montenegro</t>
-  </si>
-  <si>
-    <t> Senegal</t>
-  </si>
-  <si>
-    <t> Malaysia</t>
-  </si>
-  <si>
-    <t> Trinidad and Tobago</t>
-  </si>
-  <si>
-    <t> Mongolia</t>
-  </si>
-  <si>
-    <t> Uruguay</t>
-  </si>
-  <si>
-    <t> Honduras</t>
-  </si>
-  <si>
-    <t> Iceland</t>
-  </si>
-  <si>
-    <t> United Arab Emirates</t>
-  </si>
-  <si>
-    <t> Armenia</t>
-  </si>
-  <si>
-    <t> Puerto Rico</t>
-  </si>
-  <si>
-    <t> Bahamas</t>
-  </si>
-  <si>
-    <t> Gabon</t>
-  </si>
-  <si>
-    <t> Singapore</t>
-  </si>
-  <si>
-    <t> Indonesia</t>
-  </si>
-  <si>
-    <t> Moldova</t>
-  </si>
-  <si>
-    <t> Pakistan</t>
-  </si>
-  <si>
-    <t> Guatemala</t>
-  </si>
-  <si>
-    <t> Saudi Arabia</t>
-  </si>
-  <si>
-    <t> Vietnam</t>
-  </si>
-  <si>
-    <t> Peru</t>
-  </si>
-  <si>
-    <t> Tajikistan</t>
-  </si>
-  <si>
-    <t> Uganda</t>
-  </si>
-  <si>
-    <t> Kyrgyzstan</t>
-  </si>
-  <si>
-    <t> Cyprus</t>
-  </si>
-  <si>
-    <t> Albania</t>
-  </si>
-  <si>
-    <t> Bahrain</t>
-  </si>
-  <si>
-    <t> Eritrea</t>
-  </si>
-  <si>
-    <t> Qatar</t>
-  </si>
-  <si>
-    <t> Costa Rica</t>
-  </si>
-  <si>
-    <t> Kuwait</t>
-  </si>
-  <si>
-    <t> Mauritius</t>
-  </si>
-  <si>
-    <t> Philippines</t>
-  </si>
-  <si>
-    <t> Ivory Coast</t>
-  </si>
-  <si>
-    <t> El Salvador</t>
-  </si>
-  <si>
-    <t> Grenada</t>
-  </si>
-  <si>
-    <t> Lebanon</t>
-  </si>
-  <si>
-    <t> Syria</t>
-  </si>
-  <si>
-    <t> Turkmenistan</t>
-  </si>
-  <si>
-    <t> Fiji</t>
-  </si>
-  <si>
-    <t> Ghana</t>
-  </si>
-  <si>
-    <t> Jordan</t>
-  </si>
-  <si>
-    <t> Luxembourg</t>
-  </si>
-  <si>
-    <t> Namibia</t>
-  </si>
-  <si>
-    <t> Bermuda</t>
-  </si>
-  <si>
-    <t> Cook Islands</t>
-  </si>
-  <si>
-    <t> Guam</t>
-  </si>
-  <si>
-    <t> Iraq</t>
-  </si>
-  <si>
-    <t> Paraguay</t>
-  </si>
-  <si>
-    <t> Papua New Guinea</t>
-  </si>
-  <si>
-    <t> Samoa</t>
-  </si>
-  <si>
-    <t> Congo</t>
-  </si>
-  <si>
-    <t> Virgin Islands</t>
-  </si>
-  <si>
-    <t> Madagascar</t>
-  </si>
-  <si>
-    <t> Panama</t>
-  </si>
-  <si>
-    <t> Rwanda</t>
-  </si>
-  <si>
-    <t> Saint Kitts and Nevis</t>
-  </si>
-  <si>
-    <t> Sri Lanka</t>
-  </si>
-  <si>
-    <t> Tanzania</t>
-  </si>
-  <si>
-    <t> Zambia</t>
-  </si>
-  <si>
-    <t> Zimbabwe</t>
-  </si>
-  <si>
-    <t> Afghanistan</t>
-  </si>
-  <si>
-    <t> Andorra</t>
-  </si>
-  <si>
-    <t> Barbados</t>
-  </si>
-  <si>
-    <t> Burundi</t>
-  </si>
-  <si>
-    <t> Bosnia and Herzegovina</t>
-  </si>
-  <si>
-    <t> Bolivia</t>
-  </si>
-  <si>
-    <t> Central African Republic</t>
-  </si>
-  <si>
-    <t> Cambodia</t>
-  </si>
-  <si>
-    <t> Djibouti</t>
-  </si>
-  <si>
-    <t> Federated States of Micronesia</t>
-  </si>
-  <si>
-    <t> Guyana</t>
-  </si>
-  <si>
-    <t> Mali</t>
-  </si>
-  <si>
-    <t> Monaco</t>
-  </si>
-  <si>
-    <t> Mozambique</t>
-  </si>
-  <si>
-    <t> Myanmar</t>
-  </si>
-  <si>
-    <t> Nicaragua</t>
-  </si>
-  <si>
-    <t> Niger</t>
-  </si>
-  <si>
-    <t> Seychelles</t>
-  </si>
-  <si>
-    <t> Sudan</t>
-  </si>
-  <si>
-    <t> Togo</t>
-  </si>
-  <si>
-    <t> Antigua and Barbuda</t>
-  </si>
-  <si>
-    <t> American Samoa</t>
-  </si>
-  <si>
-    <t> Bangladesh</t>
-  </si>
-  <si>
-    <t> Benin</t>
-  </si>
-  <si>
-    <t> Burkina Faso</t>
-  </si>
-  <si>
-    <t> Cayman Islands</t>
-  </si>
-  <si>
-    <t> Haiti</t>
-  </si>
-  <si>
-    <t> Libya</t>
-  </si>
-  <si>
-    <t> Maldives</t>
-  </si>
-  <si>
-    <t> Malta</t>
-  </si>
-  <si>
-    <t> Nepal</t>
-  </si>
-  <si>
-    <t> Palestine</t>
-  </si>
-  <si>
-    <t> Palau</t>
-  </si>
-  <si>
-    <t> Suriname</t>
-  </si>
-  <si>
-    <t> Vanuatu</t>
-  </si>
-  <si>
-    <t> Aruba</t>
-  </si>
-  <si>
-    <t> Botswana</t>
-  </si>
-  <si>
-    <t> DR Congo</t>
-  </si>
-  <si>
-    <t> Guinea-Bissau</t>
-  </si>
-  <si>
-    <t> Guinea</t>
-  </si>
-  <si>
-    <t> Independent Olympic Athletes</t>
-  </si>
-  <si>
-    <t> Liberia</t>
-  </si>
-  <si>
-    <t> Saint Lucia</t>
-  </si>
-  <si>
-    <t> Lesotho</t>
-  </si>
-  <si>
-    <t> Marshall Islands</t>
-  </si>
-  <si>
-    <t> Macedonia</t>
-  </si>
-  <si>
-    <t> Oman</t>
-  </si>
-  <si>
-    <t> San Marino</t>
-  </si>
-  <si>
-    <t> Solomon Islands</t>
-  </si>
-  <si>
-    <t> Yemen</t>
-  </si>
-  <si>
-    <t> Belize</t>
-  </si>
-  <si>
-    <t> Brunei</t>
-  </si>
-  <si>
-    <t> Chad</t>
-  </si>
-  <si>
-    <t> Comoros</t>
-  </si>
-  <si>
-    <t> Cape Verde</t>
-  </si>
-  <si>
-    <t> Kiribati</t>
-  </si>
-  <si>
-    <t> Laos</t>
-  </si>
-  <si>
-    <t> Liechtenstein</t>
-  </si>
-  <si>
-    <t> Malawi</t>
-  </si>
-  <si>
-    <t> Swaziland</t>
-  </si>
-  <si>
-    <t> Tonga</t>
-  </si>
-  <si>
-    <t> Tuvalu</t>
-  </si>
-  <si>
-    <t> Saint Vincent and the Grenadines</t>
-  </si>
-  <si>
-    <t> Bhutan</t>
-  </si>
-  <si>
-    <t> Dominica</t>
-  </si>
-  <si>
-    <t> The Gambia</t>
-  </si>
-  <si>
-    <t> Equatorial Guinea</t>
-  </si>
-  <si>
-    <t> British Virgin Islands</t>
-  </si>
-  <si>
-    <t> Mauritania</t>
-  </si>
-  <si>
-    <t> Nauru</t>
-  </si>
-  <si>
-    <t> Sierra Leone</t>
-  </si>
-  <si>
-    <t> Somalia</t>
-  </si>
-  <si>
-    <t> São Tomé and Príncipe</t>
-  </si>
-  <si>
-    <t> Timor-Leste</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -638,6 +23,621 @@
   </si>
   <si>
     <t>Percentage of All Athletes</t>
+  </si>
+  <si>
+    <t>Great Britain</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Chinese Taipei</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Ivory Coast</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Cook Islands</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Virgin Islands</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Federated States of Micronesia</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>DR Congo</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Independent Olympic Athletes</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>The Gambia</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>British Virgin Islands</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>São Tomé and Príncipe</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
   </si>
 </sst>
 </file>
@@ -973,25 +973,25 @@
   <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>540</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>530</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>436</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>410</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>396</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>392</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>330</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>293</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>284</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>282</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>277</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>258</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>245</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>237</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>218</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>184</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>175</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>165</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>157</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>137</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>134</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>133</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>125</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>115</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>115</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>114</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>114</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>113</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>113</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>110</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>108</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>104</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>103</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>103</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>102</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>102</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>83</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>83</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>77</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>70</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>70</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>67</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>66</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>65</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>64</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B47">
         <v>63</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <v>62</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <v>55</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>55</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>54</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>53</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>53</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>51</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B55">
         <v>50</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B56">
         <v>47</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B57">
         <v>47</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>46</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>44</v>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>42</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B61">
         <v>42</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B62">
         <v>37</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B63">
         <v>37</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>36</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <v>35</v>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <v>35</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>35</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B68">
         <v>35</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B69">
         <v>34</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B70">
         <v>33</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B71">
         <v>33</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B72">
         <v>33</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B73">
         <v>31</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B74">
         <v>30</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B75">
         <v>30</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>29</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B77">
         <v>29</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>27</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B79">
         <v>27</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B80">
         <v>26</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B81">
         <v>25</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B82">
         <v>25</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>24</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>24</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>23</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B86">
         <v>22</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B87">
         <v>22</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>21</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>19</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B90">
         <v>19</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B91">
         <v>18</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B92">
         <v>16</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B93">
         <v>16</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B94">
         <v>16</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B95">
         <v>14</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B96">
         <v>13</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B97">
         <v>12</v>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B98">
         <v>12</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B99">
         <v>12</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B100">
         <v>12</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B101">
         <v>11</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B102">
         <v>11</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B103">
         <v>11</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B104">
         <v>11</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B105">
         <v>10</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B106">
         <v>10</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B107">
         <v>10</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B108">
         <v>10</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B109">
         <v>10</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B110">
         <v>10</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B111">
         <v>9</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B112">
         <v>9</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B113">
         <v>9</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B114">
         <v>9</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B115">
         <v>9</v>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B116">
         <v>8</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B117">
         <v>8</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B118">
         <v>8</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B119">
         <v>8</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B120">
         <v>8</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B121">
         <v>8</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B122">
         <v>8</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B123">
         <v>7</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B124">
         <v>7</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B125">
         <v>7</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B126">
         <v>7</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B127">
         <v>7</v>
@@ -2503,7 +2503,7 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B128">
         <v>7</v>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B129">
         <v>7</v>
@@ -2527,7 +2527,7 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B130">
         <v>7</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B131">
         <v>7</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B132">
         <v>7</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B133">
         <v>6</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B134">
         <v>6</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B135">
         <v>6</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B136">
         <v>6</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B137">
         <v>6</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B138">
         <v>6</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B139">
         <v>6</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B140">
         <v>6</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B141">
         <v>6</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B142">
         <v>6</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B143">
         <v>6</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B144">
         <v>6</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B145">
         <v>6</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B146">
         <v>6</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B147">
         <v>6</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B148">
         <v>6</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B149">
         <v>6</v>
@@ -2767,7 +2767,7 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B150">
         <v>6</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B151">
         <v>6</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B152">
         <v>6</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B153">
         <v>5</v>
@@ -2815,7 +2815,7 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B154">
         <v>5</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B155">
         <v>5</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B156">
         <v>5</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B157">
         <v>5</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B158">
         <v>5</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B159">
         <v>5</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B160">
         <v>5</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B161">
         <v>5</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B162">
         <v>5</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B163">
         <v>5</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B164">
         <v>5</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B165">
         <v>5</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B166">
         <v>5</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B167">
         <v>5</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B168">
         <v>4</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B169">
         <v>4</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B170">
         <v>4</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B171">
         <v>4</v>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B172">
         <v>4</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B173">
         <v>4</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B174">
         <v>4</v>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B175">
         <v>4</v>
@@ -3079,7 +3079,7 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B176">
         <v>4</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B177">
         <v>4</v>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B178">
         <v>4</v>
@@ -3115,7 +3115,7 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B179">
         <v>4</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B180">
         <v>4</v>
@@ -3139,7 +3139,7 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B181">
         <v>4</v>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B182">
         <v>4</v>
@@ -3163,7 +3163,7 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B183">
         <v>3</v>
@@ -3175,7 +3175,7 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B184">
         <v>3</v>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B185">
         <v>3</v>
@@ -3199,7 +3199,7 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B186">
         <v>3</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B187">
         <v>3</v>
@@ -3223,7 +3223,7 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B188">
         <v>3</v>
@@ -3235,7 +3235,7 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B189">
         <v>3</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B190">
         <v>3</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B191">
         <v>3</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B192">
         <v>3</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B193">
         <v>3</v>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B194">
         <v>3</v>
@@ -3307,7 +3307,7 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B195">
         <v>3</v>
@@ -3319,7 +3319,7 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B196">
         <v>2</v>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B197">
         <v>2</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B198">
         <v>2</v>
@@ -3355,7 +3355,7 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B199">
         <v>2</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B200">
         <v>2</v>
@@ -3379,7 +3379,7 @@
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B201">
         <v>2</v>
@@ -3391,7 +3391,7 @@
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B202">
         <v>2</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B203">
         <v>2</v>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B204">
         <v>2</v>
@@ -3427,7 +3427,7 @@
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B205">
         <v>2</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B206">
         <v>2</v>

</xml_diff>